<commit_message>
Ajuste de la estimacion de tiempo
</commit_message>
<xml_diff>
--- a/CSOF5101 Ingeniera de Software/TSP/RegresionLinealTSP.xlsx
+++ b/CSOF5101 Ingeniera de Software/TSP/RegresionLinealTSP.xlsx
@@ -345,11 +345,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="50788992"/>
-        <c:axId val="68699264"/>
+        <c:axId val="46987904"/>
+        <c:axId val="56050816"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50788992"/>
+        <c:axId val="46987904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="600"/>
@@ -391,13 +391,13 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="68699264"/>
+        <c:crossAx val="56050816"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="50"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="68699264"/>
+        <c:axId val="56050816"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1000"/>
@@ -439,7 +439,7 @@
             <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50788992"/>
+        <c:crossAx val="46987904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -470,7 +470,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
   <c:userShapes r:id="rId1"/>
@@ -1152,7 +1152,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F26"/>
+  <dimension ref="B2:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1312,7 +1312,7 @@
         <v>313.2</v>
       </c>
     </row>
-    <row r="17" spans="2:6">
+    <row r="17" spans="2:7">
       <c r="B17" t="s">
         <v>10</v>
       </c>
@@ -1320,7 +1320,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="2:6">
+    <row r="18" spans="2:7">
       <c r="B18" t="s">
         <v>1</v>
       </c>
@@ -1329,7 +1329,7 @@
         <v>1.5674556213017752</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:7">
       <c r="B19" t="s">
         <v>0</v>
       </c>
@@ -1338,7 +1338,7 @@
         <v>27.923076923076906</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:7">
       <c r="B22" s="5">
         <v>60</v>
       </c>
@@ -1352,7 +1352,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:7">
       <c r="B23" s="5">
         <v>80</v>
       </c>
@@ -1366,7 +1366,7 @@
         <v>317</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:7">
       <c r="B24" s="5">
         <v>100</v>
       </c>
@@ -1380,7 +1380,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:7">
       <c r="B25" s="5">
         <v>120</v>
       </c>
@@ -1394,7 +1394,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:7">
       <c r="B26" s="5">
         <v>145</v>
       </c>
@@ -1406,6 +1406,18 @@
       </c>
       <c r="F26">
         <v>346</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7">
+      <c r="E28">
+        <v>934</v>
+      </c>
+      <c r="F28">
+        <v>22.19</v>
+      </c>
+      <c r="G28">
+        <f>E28/F28</f>
+        <v>42.091031996394769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>